<commit_message>
refactor: PCB design change
finished ps and bus3b Line length design
</commit_message>
<xml_diff>
--- a/doc/PinMap.xlsx
+++ b/doc/PinMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1.My_Tech_Studio\1.Project\MyOECU\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962BF1A2-0196-4CC2-9D90-4DABC6FB5F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65F3DDD-38D1-4BA3-8EA4-ACEE4830B370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RGMII!$A$2:$J$15</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="129">
   <si>
     <t>MDIO</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -505,10 +505,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>底板线长(mil)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>引脚</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -542,6 +538,18 @@
   </si>
   <si>
     <t>功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>目标线长(mil)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>目标底板线长(mil)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原底板线长(mil)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -572,12 +580,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -592,12 +624,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -901,28 +945,28 @@
         <v>114</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1384,190 +1428,394 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2198469C-83D1-45C2-BB60-C36C517A15C4}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="3" width="9.75" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.75" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="4" max="4" width="18.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.25" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>1314</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="D2" s="3">
+        <v>2127.777</v>
+      </c>
+      <c r="E2" s="3">
+        <f>D2+C2</f>
+        <v>3441.777</v>
+      </c>
+      <c r="F2" s="3">
+        <v>4069.4250000000002</v>
+      </c>
+      <c r="G2" s="4">
+        <f>F2-C2</f>
+        <v>2755.4250000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>1259.03</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="D3" s="3">
+        <v>2460.6669999999999</v>
+      </c>
+      <c r="E3" s="3">
+        <f>D3+C3</f>
+        <v>3719.6970000000001</v>
+      </c>
+      <c r="F3" s="3">
+        <v>4069.4250000000002</v>
+      </c>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G13" si="0">F3-C3</f>
+        <v>2810.3950000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>1313.48</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="D4" s="3">
+        <v>2446.5810000000001</v>
+      </c>
+      <c r="E4" s="3">
+        <f>D4+C4</f>
+        <v>3760.0610000000001</v>
+      </c>
+      <c r="F4" s="3">
+        <v>4069.4250000000002</v>
+      </c>
+      <c r="G4" s="4">
+        <f>F4-C4</f>
+        <v>2755.9450000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>1616.49</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="D5" s="3">
+        <v>2452.9349999999999</v>
+      </c>
+      <c r="E5" s="3">
+        <f>D5+C5</f>
+        <v>4069.4250000000002</v>
+      </c>
+      <c r="F5" s="3">
+        <v>4069.4250000000002</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="0"/>
+        <v>2452.9350000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>1431.49</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="D6" s="3">
+        <v>2475.8539999999998</v>
+      </c>
+      <c r="E6" s="3">
+        <f>D6+C6</f>
+        <v>3907.3440000000001</v>
+      </c>
+      <c r="F6" s="3">
+        <v>4069.4250000000002</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="0"/>
+        <v>2637.9350000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>1228.4100000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="D7" s="3">
+        <v>2296.5129999999999</v>
+      </c>
+      <c r="E7" s="3">
+        <f>D7+C7</f>
+        <v>3524.9229999999998</v>
+      </c>
+      <c r="F7" s="3">
+        <v>4069.4250000000002</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>2841.0150000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>1410.68</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="D8" s="2">
+        <v>2344.6999999999998</v>
+      </c>
+      <c r="E8" s="2">
+        <f>D8+C8</f>
+        <v>3755.38</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3755.38</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>2344.6999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>1459.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="D9" s="2">
+        <v>1895.6320000000001</v>
+      </c>
+      <c r="E9" s="2">
+        <f>D9+C9</f>
+        <v>3355.5320000000002</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3755.38</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>2295.48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>1494.78</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="D10" s="2">
+        <v>1876.527</v>
+      </c>
+      <c r="E10" s="2">
+        <f>D10+C10</f>
+        <v>3371.3069999999998</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3755.38</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>2260.6000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>1199.74</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="D11" s="2">
+        <v>2039.0050000000001</v>
+      </c>
+      <c r="E11" s="2">
+        <f>D11+C11</f>
+        <v>3238.7449999999999</v>
+      </c>
+      <c r="F11" s="2">
+        <v>3755.38</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="0"/>
+        <v>2555.6400000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>1543.44</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="D12" s="2">
+        <v>1930.127</v>
+      </c>
+      <c r="E12" s="2">
+        <f>D12+C12</f>
+        <v>3473.567</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3755.38</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>2211.94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>1352.49</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="D13" s="2">
+        <v>2339.8440000000001</v>
+      </c>
+      <c r="E13" s="2">
+        <f>D13+C13</f>
+        <v>3692.3339999999998</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3755.38</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="0"/>
+        <v>2402.8900000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="5">
         <v>3507.74</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="D14" s="5">
+        <v>2305.297</v>
+      </c>
+      <c r="E14" s="5">
+        <f>D14+C14</f>
+        <v>5813.0370000000003</v>
+      </c>
+      <c r="F14" s="5">
+        <v>6175.1659999999993</v>
+      </c>
+      <c r="G14" s="4">
+        <f>F14-C14</f>
+        <v>2667.4259999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="5">
         <v>3806.12</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2369.0459999999998</v>
+      </c>
+      <c r="E15" s="5">
+        <f>D15+C15</f>
+        <v>6175.1659999999993</v>
+      </c>
+      <c r="F15" s="5">
+        <v>6175.1659999999993</v>
+      </c>
+      <c r="G15" s="4">
+        <f>F15-C15</f>
+        <v>2369.0459999999994</v>
       </c>
     </row>
   </sheetData>
@@ -1579,10 +1827,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5862D16-B648-41F8-BC8C-6155D3A4494E}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1594,174 +1842,180 @@
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>1343.89</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>1540.72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>1335.39</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>1540.71</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>775.22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>775.22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>1488.9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>1401.12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>1265</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>1487.9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>1260.32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>1400.22</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="5">
         <v>724.86</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="5">
         <v>706.37</v>
       </c>
     </row>
@@ -1773,10 +2027,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93261651-9ACA-48CF-A58C-FEFFF0361CF5}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1788,174 +2042,180 @@
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>1235.73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>834.43</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>720.68</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>1035.8699999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>715.62</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>1039.74</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>832.76</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>704.56</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>701.95</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>701.95</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>1239.3900000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>726.65</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="5">
         <v>736.26</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="5">
         <v>733.01</v>
       </c>
     </row>
@@ -1967,10 +2227,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1D9F2-E82C-4F14-8C6B-AC0BFAD5B59E}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1982,174 +2242,180 @@
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>1160.97</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>1162.5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>1235.6300000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>1238.67</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>1152.96</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>1150.55</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>1296.0999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>2279.25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>1857.69</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>1850.24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>1294.23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>2283.65</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="5">
         <v>1030.3499999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="5">
         <v>1023.8</v>
       </c>
     </row>
@@ -2161,10 +2427,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C478F0-2364-42A2-960C-4C48C4B085CA}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2176,174 +2442,180 @@
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>456.67</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>491.41</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>545.48</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>495.19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>546.58000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>495.2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>493.22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>548.66999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>623.84</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>546.86</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>456.67</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>628.9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="5">
         <v>607.28</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="5">
         <v>610.66</v>
       </c>
     </row>
@@ -2355,10 +2627,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2A023F9-A630-40F2-90F0-68B5547D10FB}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2370,174 +2642,180 @@
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>762.59</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>907.06</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>828.35</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>1011.26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>827.66</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>1028.8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>925.11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <v>705.2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <v>1088.3900000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="4">
         <v>1081.2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="4">
         <v>763.27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="4">
         <v>701.81</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="5">
         <v>900.56</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="5">
         <v>1080.8699999999999</v>
       </c>
     </row>
@@ -2549,190 +2827,380 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8B24199-6869-4102-BECF-FF79DC2D4899}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="3" width="10.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="4" max="4" width="18" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.75" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>1161.1099999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="D2" s="3">
+        <v>2074.0410000000002</v>
+      </c>
+      <c r="E2" s="3">
+        <f>D2+C2</f>
+        <v>3235.1509999999998</v>
+      </c>
+      <c r="F2" s="3">
+        <v>3809.3469999999998</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2-C2</f>
+        <v>2648.2370000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>1370.08</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="D3" s="3">
+        <v>1702.578</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E15" si="0">D3+C3</f>
+        <v>3072.6579999999999</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3809.3469999999998</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G13" si="1">F3-C3</f>
+        <v>2439.2669999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>1163.75</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="D4" s="3">
+        <v>2071.5819999999999</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>3235.3319999999999</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3809.3469999999998</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="1"/>
+        <v>2645.5969999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>1372.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="D5" s="3">
+        <v>1716.1410000000001</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>3089.0410000000002</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3809.3469999999998</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="1"/>
+        <v>2436.4469999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>1412.02</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="D6" s="3">
+        <v>2371.4340000000002</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>3783.4540000000002</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3809.3469999999998</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="1"/>
+        <v>2397.3269999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>1414.86</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="D7" s="3">
+        <v>2394.4870000000001</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>3809.3469999999998</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3809.3469999999998</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="1"/>
+        <v>2394.4870000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>1169.32</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="D8" s="2">
+        <v>1699.56</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>2868.88</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3266.145</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="1"/>
+        <v>2096.8249999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>1066.57</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="D9" s="2">
+        <v>1759.8219999999999</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>2826.3919999999998</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3266.145</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="1"/>
+        <v>2199.5749999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>1171.8499999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="D10" s="2">
+        <v>2094.2950000000001</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>3266.145</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3266.145</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="1"/>
+        <v>2094.2950000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>1170.55</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="D11" s="2">
+        <v>1702.492</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>2873.0419999999999</v>
+      </c>
+      <c r="F11" s="2">
+        <v>3266.145</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="1"/>
+        <v>2095.5950000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>1153.25</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="D12" s="2">
+        <v>2096.4229999999998</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>3249.6729999999998</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3266.145</v>
+      </c>
+      <c r="G12" s="3">
+        <f>F12-C12</f>
+        <v>2112.895</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>901.66</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="D13" s="2">
+        <v>2204.779</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>3106.4389999999999</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3266.145</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="1"/>
+        <v>2364.4850000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="5">
         <v>1479.88</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="D14" s="5">
+        <v>2560.192</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>4040.0720000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="5">
         <v>1482.76</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2558.1390000000001</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>4040.8990000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>